<commit_message>
WOrked on qoutation analysis
</commit_message>
<xml_diff>
--- a/data/quotation_princing_analysis/INDEPENDENT CIP EVAPORATOR CIR RETURN LINE GOING TO IS 400M3 TANK - ACEPACK.xlsx
+++ b/data/quotation_princing_analysis/INDEPENDENT CIP EVAPORATOR CIR RETURN LINE GOING TO IS 400M3 TANK - ACEPACK.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\00_ML\00_Power BI\docu1\tbmc-data-management\data\quotation_princing_analysis\Ongoing\For CSV\for next cleaning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\00_ML\00_Power BI\docu1\tbmc-data-management\data\quotation_princing_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A725AC-96E7-419C-A2A7-EED31F806130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125F5093-401F-43CD-BDCA-F402974A63AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <definedName name="_5SHUTTLEBUS">#N/A</definedName>
     <definedName name="_BUS142">#N/A</definedName>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Reconcillation -Original cost'!$A$1:$O$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Reconcillation -Original cost'!$A$1:$O$1</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Sort" hidden="1">#REF!</definedName>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="119">
   <si>
     <t>UNIT</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>gal</t>
-  </si>
-  <si>
-    <t>`</t>
   </si>
   <si>
     <t>PROJECT</t>
@@ -1491,7 +1488,7 @@
   <dimension ref="A1:O109"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1514,10 +1511,10 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>0</v>
@@ -1532,22 +1529,22 @@
         <v>3</v>
       </c>
       <c r="G1" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="I1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>23</v>
       </c>
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
@@ -1564,21 +1561,21 @@
         <v>121400</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
@@ -1595,21 +1592,21 @@
         <v>20000</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
@@ -1626,21 +1623,21 @@
         <v>24000</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
@@ -1657,21 +1654,21 @@
         <v>18000</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
@@ -1688,25 +1685,23 @@
         <v>1800</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1721,21 +1716,21 @@
         <v>5000</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
@@ -1752,21 +1747,21 @@
         <v>24000</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4" t="s">
@@ -1783,21 +1778,21 @@
         <v>24000</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
@@ -1814,21 +1809,21 @@
         <v>156400</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
@@ -1845,21 +1840,21 @@
         <v>5000</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
@@ -1876,21 +1871,21 @@
         <v>9000</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="4" t="s">
@@ -1907,21 +1902,21 @@
         <v>2000</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4" t="s">
@@ -1938,21 +1933,21 @@
         <v>2000</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="4" t="s">
@@ -1969,21 +1964,21 @@
         <v>30000</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="4" t="s">
@@ -2000,21 +1995,21 @@
         <v>4000</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
@@ -2031,21 +2026,21 @@
         <v>10000</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="4" t="s">
@@ -2062,21 +2057,21 @@
         <v>20000</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="4" t="s">
@@ -2088,20 +2083,20 @@
       <c r="E19" s="19"/>
       <c r="F19" s="18"/>
       <c r="G19" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M19" s="10"/>
     </row>
     <row r="20" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="4" t="s">
@@ -2113,20 +2108,20 @@
       <c r="E20" s="20"/>
       <c r="F20" s="18"/>
       <c r="G20" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M20" s="10"/>
     </row>
     <row r="21" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="4" t="s">
@@ -2138,20 +2133,20 @@
       <c r="E21" s="20"/>
       <c r="F21" s="18"/>
       <c r="G21" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M21" s="10"/>
     </row>
     <row r="22" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="4" t="s">
@@ -2163,20 +2158,20 @@
       <c r="E22" s="20"/>
       <c r="F22" s="18"/>
       <c r="G22" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M22" s="10"/>
     </row>
     <row r="23" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="24"/>
       <c r="C23" s="4" t="s">
@@ -2193,20 +2188,20 @@
         <v>69936</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M23" s="10"/>
     </row>
     <row r="24" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="4" t="s">
@@ -2223,20 +2218,20 @@
         <v>56000</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="4" t="s">
@@ -2253,20 +2248,20 @@
         <v>29000</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M25" s="10"/>
     </row>
     <row r="26" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="24"/>
       <c r="C26" s="4" t="s">
@@ -2283,20 +2278,20 @@
         <v>12300</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M26" s="10"/>
     </row>
     <row r="27" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="4" t="s">
@@ -2313,20 +2308,20 @@
         <v>130</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="4" t="s">
@@ -2343,20 +2338,20 @@
         <v>11051.74</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M28" s="10"/>
     </row>
     <row r="29" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="24"/>
       <c r="C29" s="4" t="s">
@@ -2373,20 +2368,20 @@
         <v>4613.5</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M29" s="10"/>
     </row>
     <row r="30" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="24"/>
       <c r="C30" s="4" t="s">
@@ -2403,20 +2398,20 @@
         <v>5700</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M30" s="10"/>
     </row>
     <row r="31" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="4" t="s">
@@ -2433,20 +2428,20 @@
         <v>2600</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M31" s="10"/>
     </row>
     <row r="32" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="24"/>
       <c r="C32" s="4" t="s">
@@ -2463,20 +2458,20 @@
         <v>5200</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M32" s="10"/>
     </row>
     <row r="33" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="4" t="s">
@@ -2488,20 +2483,20 @@
       <c r="E33" s="20"/>
       <c r="F33" s="18"/>
       <c r="G33" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M33" s="10"/>
     </row>
     <row r="34" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="24"/>
       <c r="C34" s="4" t="s">
@@ -2518,20 +2513,20 @@
         <v>11656</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M34" s="10"/>
     </row>
     <row r="35" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="24"/>
       <c r="C35" s="4" t="s">
@@ -2548,20 +2543,20 @@
         <v>1500</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M35" s="10"/>
     </row>
     <row r="36" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="24"/>
       <c r="C36" s="4" t="s">
@@ -2578,20 +2573,20 @@
         <v>2300</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M36" s="10"/>
     </row>
     <row r="37" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="24"/>
       <c r="C37" s="4" t="s">
@@ -2603,20 +2598,20 @@
       <c r="E37" s="20"/>
       <c r="F37" s="18"/>
       <c r="G37" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M37" s="10"/>
     </row>
     <row r="38" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="24"/>
       <c r="C38" s="4" t="s">
@@ -2633,20 +2628,20 @@
         <v>11656</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I38" s="5"/>
       <c r="J38" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M38" s="10"/>
     </row>
     <row r="39" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39" s="24"/>
       <c r="C39" s="4" t="s">
@@ -2663,20 +2658,20 @@
         <v>27384</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M39" s="10"/>
     </row>
     <row r="40" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40" s="24"/>
       <c r="C40" s="4" t="s">
@@ -2693,20 +2688,20 @@
         <v>35000</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M40" s="10"/>
     </row>
     <row r="41" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="4" t="s">
@@ -2723,20 +2718,20 @@
         <v>26500</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I41" s="5"/>
       <c r="J41" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M41" s="10"/>
     </row>
     <row r="42" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42" s="24"/>
       <c r="C42" s="4" t="s">
@@ -2753,20 +2748,20 @@
         <v>2300</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M42" s="10"/>
     </row>
     <row r="43" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" s="24"/>
       <c r="C43" s="4" t="s">
@@ -2778,20 +2773,20 @@
       <c r="E43" s="20"/>
       <c r="F43" s="18"/>
       <c r="G43" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M43" s="10"/>
     </row>
     <row r="44" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" s="24"/>
       <c r="C44" s="4" t="s">
@@ -2808,20 +2803,20 @@
         <v>11656</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M44" s="10"/>
     </row>
     <row r="45" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45" s="24"/>
       <c r="C45" s="4" t="s">
@@ -2838,20 +2833,20 @@
         <v>27384</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M45" s="10"/>
     </row>
     <row r="46" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" s="24"/>
       <c r="C46" s="4" t="s">
@@ -2868,20 +2863,20 @@
         <v>26500</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M46" s="10"/>
     </row>
     <row r="47" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="4" t="s">
@@ -2898,20 +2893,20 @@
         <v>2300</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M47" s="10"/>
     </row>
     <row r="48" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B48" s="24"/>
       <c r="C48" s="4" t="s">
@@ -2923,20 +2918,20 @@
       <c r="E48" s="20"/>
       <c r="F48" s="18"/>
       <c r="G48" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M48" s="10"/>
     </row>
     <row r="49" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B49" s="24"/>
       <c r="C49" s="4" t="s">
@@ -2953,20 +2948,20 @@
         <v>27384</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M49" s="10"/>
     </row>
     <row r="50" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50" s="24"/>
       <c r="C50" s="4" t="s">
@@ -2983,20 +2978,20 @@
         <v>1500</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M50" s="10"/>
     </row>
     <row r="51" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B51" s="24"/>
       <c r="C51" s="4" t="s">
@@ -3013,20 +3008,20 @@
         <v>11656</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M51" s="10"/>
     </row>
     <row r="52" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B52" s="24"/>
       <c r="C52" s="4" t="s">
@@ -3043,20 +3038,20 @@
         <v>6900</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I52" s="5"/>
       <c r="J52" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M52" s="10"/>
     </row>
     <row r="53" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B53" s="24"/>
       <c r="C53" s="4" t="s">
@@ -3073,20 +3068,20 @@
         <v>26500</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M53" s="10"/>
     </row>
     <row r="54" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B54" s="24"/>
       <c r="C54" s="4" t="s">
@@ -3098,24 +3093,24 @@
       <c r="E54" s="20"/>
       <c r="F54" s="18"/>
       <c r="G54" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I54" s="5"/>
       <c r="J54" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M54" s="10"/>
     </row>
     <row r="55" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B55" s="24"/>
       <c r="C55" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D55" s="17">
         <v>10</v>
@@ -3128,20 +3123,20 @@
         <v>219000</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I55" s="5"/>
       <c r="J55" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M55" s="10"/>
     </row>
     <row r="56" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B56" s="24"/>
       <c r="C56" s="4" t="s">
@@ -3158,20 +3153,20 @@
         <v>9855</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M56" s="10"/>
     </row>
     <row r="57" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57" s="24"/>
       <c r="C57" s="4" t="s">
@@ -3188,20 +3183,20 @@
         <v>7250</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I57" s="5"/>
       <c r="J57" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M57" s="10"/>
     </row>
     <row r="58" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B58" s="24"/>
       <c r="C58" s="4" t="s">
@@ -3218,20 +3213,20 @@
         <v>4600</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I58" s="5"/>
       <c r="J58" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M58" s="10"/>
     </row>
     <row r="59" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B59" s="24"/>
       <c r="C59" s="4" t="s">
@@ -3248,20 +3243,20 @@
         <v>7320</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M59" s="10"/>
     </row>
     <row r="60" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B60" s="24"/>
       <c r="C60" s="4" t="s">
@@ -3278,20 +3273,20 @@
         <v>116560</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I60" s="5"/>
       <c r="J60" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M60" s="10"/>
     </row>
     <row r="61" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" s="24"/>
       <c r="C61" s="4" t="s">
@@ -3308,20 +3303,20 @@
         <v>5360</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I61" s="5"/>
       <c r="J61" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M61" s="10"/>
     </row>
     <row r="62" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" s="24"/>
       <c r="C62" s="4" t="s">
@@ -3333,20 +3328,20 @@
       <c r="E62" s="20"/>
       <c r="F62" s="18"/>
       <c r="G62" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I62" s="5"/>
       <c r="J62" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M62" s="10"/>
     </row>
     <row r="63" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B63" s="24"/>
       <c r="C63" s="4" t="s">
@@ -3358,20 +3353,20 @@
       <c r="E63" s="20"/>
       <c r="F63" s="18"/>
       <c r="G63" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I63" s="5"/>
       <c r="J63" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M63" s="10"/>
     </row>
     <row r="64" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B64" s="24"/>
       <c r="C64" s="4" t="s">
@@ -3383,20 +3378,20 @@
       <c r="E64" s="20"/>
       <c r="F64" s="18"/>
       <c r="G64" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I64" s="5"/>
       <c r="J64" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M64" s="10"/>
     </row>
     <row r="65" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B65" s="24"/>
       <c r="C65" s="4" t="s">
@@ -3408,20 +3403,20 @@
       <c r="E65" s="20"/>
       <c r="F65" s="18"/>
       <c r="G65" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I65" s="5"/>
       <c r="J65" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M65" s="10"/>
     </row>
     <row r="66" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B66" s="24"/>
       <c r="C66" s="4" t="s">
@@ -3438,24 +3433,24 @@
         <v>69936</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I66" s="5"/>
       <c r="J66" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M66" s="10"/>
     </row>
     <row r="67" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B67" s="24"/>
       <c r="C67" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D67" s="17">
         <v>13</v>
@@ -3468,24 +3463,24 @@
         <v>284700</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I67" s="5"/>
       <c r="J67" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M67" s="10"/>
     </row>
     <row r="68" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B68" s="24"/>
       <c r="C68" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D68" s="17">
         <v>2</v>
@@ -3498,20 +3493,20 @@
         <v>9400</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I68" s="5"/>
       <c r="J68" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M68" s="10"/>
     </row>
     <row r="69" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B69" s="24"/>
       <c r="C69" s="4" t="s">
@@ -3528,20 +3523,20 @@
         <v>13140</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I69" s="5"/>
       <c r="J69" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M69" s="10"/>
     </row>
     <row r="70" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B70" s="24"/>
       <c r="C70" s="4" t="s">
@@ -3558,20 +3553,20 @@
         <v>28750</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I70" s="5"/>
       <c r="J70" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M70" s="10"/>
     </row>
     <row r="71" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B71" s="24"/>
       <c r="C71" s="4" t="s">
@@ -3588,20 +3583,20 @@
         <v>17080</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I71" s="5"/>
       <c r="J71" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M71" s="10"/>
     </row>
     <row r="72" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B72" s="24"/>
       <c r="C72" s="4" t="s">
@@ -3618,20 +3613,20 @@
         <v>1800</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I72" s="5"/>
       <c r="J72" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M72" s="10"/>
     </row>
     <row r="73" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B73" s="24"/>
       <c r="C73" s="4" t="s">
@@ -3648,20 +3643,20 @@
         <v>7250</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I73" s="5"/>
       <c r="J73" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M73" s="10"/>
     </row>
     <row r="74" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B74" s="24"/>
       <c r="C74" s="4" t="s">
@@ -3678,20 +3673,20 @@
         <v>8240</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I74" s="5"/>
       <c r="J74" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M74" s="10"/>
     </row>
     <row r="75" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B75" s="24"/>
       <c r="C75" s="4" t="s">
@@ -3703,20 +3698,20 @@
       <c r="E75" s="20"/>
       <c r="F75" s="18"/>
       <c r="G75" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I75" s="5"/>
       <c r="J75" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M75" s="10"/>
     </row>
     <row r="76" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B76" s="24"/>
       <c r="C76" s="4" t="s">
@@ -3733,20 +3728,20 @@
         <v>3680</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I76" s="5"/>
       <c r="J76" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M76" s="10"/>
     </row>
     <row r="77" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B77" s="24"/>
       <c r="C77" s="4" t="s">
@@ -3763,24 +3758,24 @@
         <v>1184.44</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M77" s="10"/>
     </row>
     <row r="78" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B78" s="24"/>
       <c r="C78" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D78" s="17">
         <v>6</v>
@@ -3793,20 +3788,20 @@
         <v>22200</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M78" s="10"/>
     </row>
     <row r="79" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B79" s="24"/>
       <c r="C79" s="4" t="s">
@@ -3823,20 +3818,20 @@
         <v>600</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I79" s="5"/>
       <c r="J79" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M79" s="10"/>
     </row>
     <row r="80" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B80" s="24"/>
       <c r="C80" s="4" t="s">
@@ -3851,20 +3846,20 @@
         <v>0</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I80" s="5"/>
       <c r="J80" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M80" s="10"/>
     </row>
     <row r="81" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B81" s="24"/>
       <c r="C81" s="4" t="s">
@@ -3881,20 +3876,20 @@
         <v>850</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I81" s="5"/>
       <c r="J81" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M81" s="10"/>
     </row>
     <row r="82" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B82" s="24"/>
       <c r="C82" s="4" t="s">
@@ -3911,20 +3906,20 @@
         <v>5000</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I82" s="5"/>
       <c r="J82" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M82" s="10"/>
     </row>
     <row r="83" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B83" s="11"/>
       <c r="C83" s="4" t="s">
@@ -3941,20 +3936,20 @@
         <v>4200</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I83" s="5"/>
       <c r="J83" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M83" s="10"/>
     </row>
     <row r="84" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B84" s="11"/>
       <c r="C84" s="4" t="s">
@@ -3971,20 +3966,20 @@
         <v>13500</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I84" s="5"/>
       <c r="J84" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M84" s="10"/>
     </row>
     <row r="85" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B85" s="11"/>
       <c r="C85" s="4" t="s">
@@ -4001,20 +3996,20 @@
         <v>13500</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I85" s="5"/>
       <c r="J85" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M85" s="10"/>
     </row>
     <row r="86" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B86" s="11"/>
       <c r="C86" s="4" t="s">
@@ -4031,20 +4026,20 @@
         <v>4200</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I86" s="5"/>
       <c r="J86" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M86" s="10"/>
     </row>
     <row r="87" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B87" s="11"/>
       <c r="C87" s="4" t="s">
@@ -4061,20 +4056,20 @@
         <v>1530</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I87" s="5"/>
       <c r="J87" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M87" s="10"/>
     </row>
     <row r="88" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B88" s="11"/>
       <c r="C88" s="4" t="s">
@@ -4091,20 +4086,20 @@
         <v>12500</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I88" s="5"/>
       <c r="J88" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M88" s="10"/>
     </row>
     <row r="89" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B89" s="11"/>
       <c r="C89" s="4" t="s">
@@ -4121,20 +4116,20 @@
         <v>3150</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I89" s="5"/>
       <c r="J89" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M89" s="10"/>
     </row>
     <row r="90" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B90" s="11"/>
       <c r="C90" s="4" t="s">
@@ -4151,20 +4146,20 @@
         <v>250</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I90" s="5"/>
       <c r="J90" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M90" s="10"/>
     </row>
     <row r="91" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B91" s="11"/>
       <c r="C91" s="4" t="s">
@@ -4181,20 +4176,20 @@
         <v>105000</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I91" s="5"/>
       <c r="J91" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M91" s="10"/>
     </row>
     <row r="92" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="4" t="s">
@@ -4211,20 +4206,20 @@
         <v>4300</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I92" s="5"/>
       <c r="J92" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M92" s="10"/>
     </row>
     <row r="93" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B93" s="11"/>
       <c r="C93" s="4" t="s">
@@ -4241,20 +4236,20 @@
         <v>1000</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I93" s="5"/>
       <c r="J93" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M93" s="10"/>
     </row>
     <row r="94" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B94" s="11"/>
       <c r="C94" s="4" t="s">
@@ -4271,20 +4266,20 @@
         <v>650</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I94" s="5"/>
       <c r="J94" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M94" s="10"/>
     </row>
     <row r="95" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B95" s="11"/>
       <c r="C95" s="4" t="s">
@@ -4301,20 +4296,20 @@
         <v>650</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I95" s="5"/>
       <c r="J95" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M95" s="10"/>
     </row>
     <row r="96" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B96" s="11"/>
       <c r="C96" s="4" t="s">
@@ -4331,20 +4326,20 @@
         <v>4100</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I96" s="5"/>
       <c r="J96" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M96" s="10"/>
     </row>
     <row r="97" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B97" s="11"/>
       <c r="C97" s="4" t="s">
@@ -4361,20 +4356,20 @@
         <v>1300</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I97" s="5"/>
       <c r="J97" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M97" s="10"/>
     </row>
     <row r="98" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B98" s="11"/>
       <c r="C98" s="4" t="s">
@@ -4391,20 +4386,20 @@
         <v>1380</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I98" s="5"/>
       <c r="J98" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M98" s="10"/>
     </row>
     <row r="99" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B99" s="11"/>
       <c r="C99" s="4" t="s">
@@ -4421,20 +4416,20 @@
         <v>17121</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H99" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I99" s="5"/>
       <c r="J99" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M99" s="10"/>
     </row>
     <row r="100" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B100" s="11">
         <v>1</v>
@@ -4453,20 +4448,20 @@
         <v>15381.24</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I100" s="5"/>
       <c r="J100" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M100" s="10"/>
     </row>
     <row r="101" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B101" s="11">
         <v>1</v>
@@ -4485,20 +4480,20 @@
         <v>67824.799999999988</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I101" s="5"/>
       <c r="J101" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M101" s="10"/>
     </row>
     <row r="102" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B102" s="11">
         <v>1</v>
@@ -4517,20 +4512,20 @@
         <v>47640</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I102" s="5"/>
       <c r="J102" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M102" s="10"/>
     </row>
     <row r="103" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B103" s="11">
         <v>1</v>
@@ -4549,20 +4544,20 @@
         <v>59944</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I103" s="5"/>
       <c r="J103" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M103" s="10"/>
     </row>
     <row r="104" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B104" s="11">
         <v>1</v>
@@ -4581,20 +4576,20 @@
         <v>59944</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I104" s="5"/>
       <c r="J104" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M104" s="10"/>
     </row>
     <row r="105" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B105" s="11">
         <v>2</v>
@@ -4613,20 +4608,20 @@
         <v>130189.59999999999</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I105" s="5"/>
       <c r="J105" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M105" s="10"/>
     </row>
     <row r="106" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B106" s="11">
         <v>3</v>
@@ -4644,20 +4639,20 @@
         <v>156020.4</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I106" s="5"/>
       <c r="J106" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M106" s="10"/>
     </row>
     <row r="107" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B107" s="11">
         <v>7</v>
@@ -4675,20 +4670,20 @@
         <v>288894.40000000002</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I107" s="5"/>
       <c r="J107" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M107" s="10"/>
     </row>
     <row r="108" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B108" s="4">
         <v>1</v>
@@ -4707,19 +4702,20 @@
         <v>36445.199999999997</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I108" s="5"/>
       <c r="J108" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M108" s="10"/>
     </row>
     <row r="109" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <autoFilter ref="A1:O1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>
   <pageSetup paperSize="8" scale="42" orientation="portrait" r:id="rId1"/>
@@ -4779,7 +4775,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Worked on some data
</commit_message>
<xml_diff>
--- a/data/quotation_princing_analysis/INDEPENDENT CIP EVAPORATOR CIR RETURN LINE GOING TO IS 400M3 TANK - ACEPACK.xlsx
+++ b/data/quotation_princing_analysis/INDEPENDENT CIP EVAPORATOR CIR RETURN LINE GOING TO IS 400M3 TANK - ACEPACK.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francis\00_ML\00_Power BI\docu1\tbmc-data-management\data\quotation_princing_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PHTadenaFr\Documents\tbmc-data-management\data\quotation_princing_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125F5093-401F-43CD-BDCA-F402974A63AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Reconcillation -Original cost" sheetId="10" r:id="rId1"/>
@@ -34,7 +33,7 @@
     <definedName name="MACHINETOOLS">#N/A</definedName>
     <definedName name="Months">[1]Sheet5!$A$1:$B$13</definedName>
     <definedName name="past" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Reconcillation -Original cost'!$A$1:$J$108</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Reconcillation -Original cost'!$A$1:$J$88</definedName>
     <definedName name="Print_Area_MI">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Reconcillation -Original cost'!$1:$1</definedName>
     <definedName name="RELOCAFETERIA">#N/A</definedName>
@@ -42,7 +41,7 @@
     <definedName name="REPLROOFPREP">#N/A</definedName>
     <definedName name="YARDGOAT">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="119">
   <si>
     <t>UNIT</t>
   </si>
@@ -422,11 +421,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.00_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.00_)"/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -887,9 +886,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="38" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -901,13 +900,13 @@
     <xf numFmtId="10" fontId="10" fillId="23" borderId="6" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -918,7 +917,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -927,13 +926,13 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="26" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -942,7 +941,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1013,33 +1012,44 @@
     <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Comma" xfId="28" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Currency 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Comma 2" xfId="29"/>
+    <cellStyle name="Currency 2" xfId="30"/>
     <cellStyle name="Explanatory Text" xfId="31" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="32" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Grey" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Grey" xfId="33"/>
     <cellStyle name="Heading 1" xfId="34" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="35" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="36" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="37" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Input" xfId="38" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Input [yellow]" xfId="39" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Input [yellow]" xfId="39"/>
     <cellStyle name="Linked Cell" xfId="40" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="41" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal - Style1" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Normal 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Normal_CDOF-EN-F-07-001 Technical Purchase Requisition Form_ENGG-00520-WAREHOUSE FLOORING REPAIR" xfId="43" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal - Style1" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="52"/>
+    <cellStyle name="Normal_CDOF-EN-F-07-001 Technical Purchase Requisition Form_ENGG-00520-WAREHOUSE FLOORING REPAIR" xfId="43"/>
     <cellStyle name="Note" xfId="44" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="45" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent [2]" xfId="46" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Percent 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Style 1" xfId="48" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Percent [2]" xfId="46"/>
+    <cellStyle name="Percent 2" xfId="47"/>
+    <cellStyle name="Style 1" xfId="48"/>
     <cellStyle name="Title" xfId="49" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="50" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="51" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1058,7 +1068,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="dcf-ror compressed form"/>
@@ -1199,9 +1209,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1239,9 +1249,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1276,7 +1286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1311,7 +1321,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1484,32 +1494,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O89"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="101.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="101.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="12" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="86.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="22.33203125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="4.5546875" style="12" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="4.6640625" style="13" customWidth="1"/>
-    <col min="14" max="15" width="3.5546875" style="13" customWidth="1"/>
-    <col min="16" max="16384" width="3.5546875" style="12"/>
+    <col min="4" max="4" width="11.5703125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="86.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="22.28515625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="13" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="13" customWidth="1"/>
+    <col min="14" max="15" width="3.5703125" style="13" customWidth="1"/>
+    <col min="16" max="16384" width="3.5703125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>29</v>
       </c>
@@ -1542,7 +1552,7 @@
       </c>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
@@ -1573,7 +1583,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
@@ -1604,7 +1614,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
@@ -1635,7 +1645,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>33</v>
       </c>
@@ -1666,7 +1676,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>34</v>
       </c>
@@ -1697,7 +1707,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>35</v>
       </c>
@@ -1728,7 +1738,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>36</v>
       </c>
@@ -1759,7 +1769,7 @@
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
@@ -1790,7 +1800,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>38</v>
       </c>
@@ -1821,7 +1831,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>39</v>
       </c>
@@ -1852,7 +1862,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>40</v>
       </c>
@@ -1883,7 +1893,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>41</v>
       </c>
@@ -1914,7 +1924,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>42</v>
       </c>
@@ -1945,7 +1955,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>43</v>
       </c>
@@ -1976,7 +1986,7 @@
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>44</v>
       </c>
@@ -2007,7 +2017,7 @@
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
     </row>
-    <row r="17" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>45</v>
       </c>
@@ -2038,7 +2048,7 @@
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
     </row>
-    <row r="18" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>46</v>
       </c>
@@ -2069,7 +2079,7 @@
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
     </row>
-    <row r="19" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>47</v>
       </c>
@@ -2094,7 +2104,7 @@
       </c>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>48</v>
       </c>
@@ -2119,7 +2129,7 @@
       </c>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>49</v>
       </c>
@@ -2144,7 +2154,7 @@
       </c>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>50</v>
       </c>
@@ -2169,7 +2179,7 @@
       </c>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>51</v>
       </c>
@@ -2178,14 +2188,14 @@
         <v>17</v>
       </c>
       <c r="D23" s="17">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E23" s="20">
         <v>11656</v>
       </c>
       <c r="F23" s="18">
         <f t="shared" ref="F23:F32" si="3">E23*D23</f>
-        <v>69936</v>
+        <v>186496</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>118</v>
@@ -2199,7 +2209,7 @@
       </c>
       <c r="M23" s="10"/>
     </row>
-    <row r="24" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>52</v>
       </c>
@@ -2229,7 +2239,7 @@
       </c>
       <c r="M24" s="10"/>
     </row>
-    <row r="25" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>53</v>
       </c>
@@ -2238,14 +2248,14 @@
         <v>6</v>
       </c>
       <c r="D25" s="17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25" s="20">
         <v>7250</v>
       </c>
       <c r="F25" s="18">
         <f t="shared" si="3"/>
-        <v>29000</v>
+        <v>43500</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>118</v>
@@ -2259,7 +2269,7 @@
       </c>
       <c r="M25" s="10"/>
     </row>
-    <row r="26" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>54</v>
       </c>
@@ -2289,7 +2299,7 @@
       </c>
       <c r="M26" s="10"/>
     </row>
-    <row r="27" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>55</v>
       </c>
@@ -2319,7 +2329,7 @@
       </c>
       <c r="M27" s="10"/>
     </row>
-    <row r="28" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>56</v>
       </c>
@@ -2349,7 +2359,7 @@
       </c>
       <c r="M28" s="10"/>
     </row>
-    <row r="29" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>57</v>
       </c>
@@ -2379,7 +2389,7 @@
       </c>
       <c r="M29" s="10"/>
     </row>
-    <row r="30" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>58</v>
       </c>
@@ -2409,7 +2419,7 @@
       </c>
       <c r="M30" s="10"/>
     </row>
-    <row r="31" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>59</v>
       </c>
@@ -2439,7 +2449,7 @@
       </c>
       <c r="M31" s="10"/>
     </row>
-    <row r="32" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>60</v>
       </c>
@@ -2448,14 +2458,14 @@
         <v>5</v>
       </c>
       <c r="D32" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E32" s="20">
         <v>5200</v>
       </c>
       <c r="F32" s="18">
         <f t="shared" si="3"/>
-        <v>5200</v>
+        <v>20800</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>118</v>
@@ -2469,7 +2479,7 @@
       </c>
       <c r="M32" s="10"/>
     </row>
-    <row r="33" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>61</v>
       </c>
@@ -2478,7 +2488,7 @@
         <v>6</v>
       </c>
       <c r="D33" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="18"/>
@@ -2494,7 +2504,7 @@
       </c>
       <c r="M33" s="10"/>
     </row>
-    <row r="34" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>62</v>
       </c>
@@ -2503,14 +2513,14 @@
         <v>17</v>
       </c>
       <c r="D34" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E34" s="20">
         <v>11656</v>
       </c>
       <c r="F34" s="18">
         <f>E34*D34</f>
-        <v>11656</v>
+        <v>46624</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>118</v>
@@ -2524,7 +2534,7 @@
       </c>
       <c r="M34" s="10"/>
     </row>
-    <row r="35" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>63</v>
       </c>
@@ -2554,7 +2564,7 @@
       </c>
       <c r="M35" s="10"/>
     </row>
-    <row r="36" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>64</v>
       </c>
@@ -2563,14 +2573,14 @@
         <v>6</v>
       </c>
       <c r="D36" s="17">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E36" s="20">
         <v>1150</v>
       </c>
       <c r="F36" s="18">
         <f>E36*D36</f>
-        <v>2300</v>
+        <v>16100</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>118</v>
@@ -2584,19 +2594,24 @@
       </c>
       <c r="M36" s="10"/>
     </row>
-    <row r="37" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B37" s="24"/>
       <c r="C37" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D37" s="17">
-        <v>1</v>
-      </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="18"/>
+        <v>3</v>
+      </c>
+      <c r="E37" s="20">
+        <v>27384</v>
+      </c>
+      <c r="F37" s="18">
+        <f>E37*D37</f>
+        <v>82152</v>
+      </c>
       <c r="G37" s="5" t="s">
         <v>118</v>
       </c>
@@ -2609,23 +2624,23 @@
       </c>
       <c r="M37" s="10"/>
     </row>
-    <row r="38" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B38" s="24"/>
       <c r="C38" s="4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D38" s="17">
         <v>1</v>
       </c>
       <c r="E38" s="20">
-        <v>11656</v>
+        <v>35000</v>
       </c>
       <c r="F38" s="18">
         <f>E38*D38</f>
-        <v>11656</v>
+        <v>35000</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>118</v>
@@ -2639,23 +2654,23 @@
       </c>
       <c r="M38" s="10"/>
     </row>
-    <row r="39" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B39" s="24"/>
       <c r="C39" s="4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D39" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E39" s="20">
-        <v>27384</v>
+        <v>26500</v>
       </c>
       <c r="F39" s="18">
         <f>E39*D39</f>
-        <v>27384</v>
+        <v>79500</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>118</v>
@@ -2669,9 +2684,9 @@
       </c>
       <c r="M39" s="10"/>
     </row>
-    <row r="40" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B40" s="24"/>
       <c r="C40" s="4" t="s">
@@ -2680,13 +2695,8 @@
       <c r="D40" s="17">
         <v>1</v>
       </c>
-      <c r="E40" s="20">
-        <v>35000</v>
-      </c>
-      <c r="F40" s="18">
-        <f>E40*D40</f>
-        <v>35000</v>
-      </c>
+      <c r="E40" s="20"/>
+      <c r="F40" s="18"/>
       <c r="G40" s="5" t="s">
         <v>118</v>
       </c>
@@ -2699,9 +2709,9 @@
       </c>
       <c r="M40" s="10"/>
     </row>
-    <row r="41" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="4" t="s">
@@ -2711,11 +2721,11 @@
         <v>1</v>
       </c>
       <c r="E41" s="20">
-        <v>26500</v>
+        <v>1500</v>
       </c>
       <c r="F41" s="18">
         <f>E41*D41</f>
-        <v>26500</v>
+        <v>1500</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>118</v>
@@ -2729,24 +2739,19 @@
       </c>
       <c r="M41" s="10"/>
     </row>
-    <row r="42" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B42" s="24"/>
       <c r="C42" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="17">
-        <v>2</v>
-      </c>
-      <c r="E42" s="20">
-        <v>1150</v>
-      </c>
-      <c r="F42" s="18">
-        <f>E42*D42</f>
-        <v>2300</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E42" s="20"/>
+      <c r="F42" s="18"/>
       <c r="G42" s="5" t="s">
         <v>118</v>
       </c>
@@ -2759,19 +2764,24 @@
       </c>
       <c r="M42" s="10"/>
     </row>
-    <row r="43" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B43" s="24"/>
       <c r="C43" s="4" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D43" s="17">
-        <v>1</v>
-      </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="18"/>
+        <v>10</v>
+      </c>
+      <c r="E43" s="18">
+        <v>21900</v>
+      </c>
+      <c r="F43" s="18">
+        <f t="shared" ref="F43:F45" si="4">E43*D43</f>
+        <v>219000</v>
+      </c>
       <c r="G43" s="5" t="s">
         <v>118</v>
       </c>
@@ -2784,23 +2794,23 @@
       </c>
       <c r="M43" s="10"/>
     </row>
-    <row r="44" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B44" s="24"/>
       <c r="C44" s="4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D44" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E44" s="20">
-        <v>11656</v>
+        <v>3285</v>
       </c>
       <c r="F44" s="18">
-        <f>E44*D44</f>
-        <v>11656</v>
+        <f t="shared" si="4"/>
+        <v>9855</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>118</v>
@@ -2814,23 +2824,23 @@
       </c>
       <c r="M44" s="10"/>
     </row>
-    <row r="45" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B45" s="24"/>
       <c r="C45" s="4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D45" s="17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E45" s="20">
-        <v>27384</v>
+        <v>1220</v>
       </c>
       <c r="F45" s="18">
-        <f>E45*D45</f>
-        <v>27384</v>
+        <f t="shared" si="4"/>
+        <v>7320</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>118</v>
@@ -2844,9 +2854,9 @@
       </c>
       <c r="M45" s="10"/>
     </row>
-    <row r="46" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B46" s="24"/>
       <c r="C46" s="4" t="s">
@@ -2855,13 +2865,8 @@
       <c r="D46" s="17">
         <v>1</v>
       </c>
-      <c r="E46" s="20">
-        <v>26500</v>
-      </c>
-      <c r="F46" s="18">
-        <f>E46*D46</f>
-        <v>26500</v>
-      </c>
+      <c r="E46" s="20"/>
+      <c r="F46" s="18"/>
       <c r="G46" s="5" t="s">
         <v>118</v>
       </c>
@@ -2874,24 +2879,19 @@
       </c>
       <c r="M46" s="10"/>
     </row>
-    <row r="47" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="17">
-        <v>2</v>
-      </c>
-      <c r="E47" s="20">
-        <v>1150</v>
-      </c>
-      <c r="F47" s="18">
-        <f>E47*D47</f>
-        <v>2300</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E47" s="20"/>
+      <c r="F47" s="18"/>
       <c r="G47" s="5" t="s">
         <v>118</v>
       </c>
@@ -2904,9 +2904,9 @@
       </c>
       <c r="M47" s="10"/>
     </row>
-    <row r="48" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B48" s="24"/>
       <c r="C48" s="4" t="s">
@@ -2929,23 +2929,23 @@
       </c>
       <c r="M48" s="10"/>
     </row>
-    <row r="49" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B49" s="24"/>
       <c r="C49" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E49" s="20">
-        <v>27384</v>
+        <v>11656</v>
       </c>
       <c r="F49" s="18">
-        <f>E49*D49</f>
-        <v>27384</v>
+        <f t="shared" ref="F49:F55" si="5">E49*D49</f>
+        <v>69936</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>118</v>
@@ -2959,23 +2959,23 @@
       </c>
       <c r="M49" s="10"/>
     </row>
-    <row r="50" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B50" s="24"/>
       <c r="C50" s="4" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D50" s="17">
-        <v>1</v>
-      </c>
-      <c r="E50" s="20">
-        <v>1500</v>
+        <v>13</v>
+      </c>
+      <c r="E50" s="18">
+        <v>21900</v>
       </c>
       <c r="F50" s="18">
-        <f>E50*D50</f>
-        <v>1500</v>
+        <f t="shared" si="5"/>
+        <v>284700</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>118</v>
@@ -2989,23 +2989,23 @@
       </c>
       <c r="M50" s="10"/>
     </row>
-    <row r="51" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B51" s="24"/>
       <c r="C51" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D51" s="17">
-        <v>1</v>
-      </c>
-      <c r="E51" s="20">
-        <v>11656</v>
+        <v>2</v>
+      </c>
+      <c r="E51" s="18">
+        <v>4700</v>
       </c>
       <c r="F51" s="18">
-        <f>E51*D51</f>
-        <v>11656</v>
+        <f t="shared" si="5"/>
+        <v>9400</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>118</v>
@@ -3019,23 +3019,23 @@
       </c>
       <c r="M51" s="10"/>
     </row>
-    <row r="52" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B52" s="24"/>
       <c r="C52" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E52" s="20">
-        <v>1150</v>
+        <v>3285</v>
       </c>
       <c r="F52" s="18">
-        <f>E52*D52</f>
-        <v>6900</v>
+        <f t="shared" si="5"/>
+        <v>13140</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>118</v>
@@ -3049,23 +3049,23 @@
       </c>
       <c r="M52" s="10"/>
     </row>
-    <row r="53" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B53" s="24"/>
       <c r="C53" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="17">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="E53" s="20">
-        <v>26500</v>
+        <v>1150</v>
       </c>
       <c r="F53" s="18">
-        <f>E53*D53</f>
-        <v>26500</v>
+        <f t="shared" si="5"/>
+        <v>28750</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>118</v>
@@ -3079,19 +3079,24 @@
       </c>
       <c r="M53" s="10"/>
     </row>
-    <row r="54" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B54" s="24"/>
       <c r="C54" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="17">
-        <v>1</v>
-      </c>
-      <c r="E54" s="20"/>
-      <c r="F54" s="18"/>
+        <v>14</v>
+      </c>
+      <c r="E54" s="20">
+        <v>1220</v>
+      </c>
+      <c r="F54" s="18">
+        <f t="shared" si="5"/>
+        <v>17080</v>
+      </c>
       <c r="G54" s="5" t="s">
         <v>118</v>
       </c>
@@ -3104,23 +3109,23 @@
       </c>
       <c r="M54" s="10"/>
     </row>
-    <row r="55" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B55" s="24"/>
       <c r="C55" s="4" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D55" s="17">
         <v>10</v>
       </c>
-      <c r="E55" s="18">
-        <v>21900</v>
+      <c r="E55" s="20">
+        <v>180</v>
       </c>
       <c r="F55" s="18">
-        <f t="shared" ref="F55:F61" si="4">E55*D55</f>
-        <v>219000</v>
+        <f t="shared" si="5"/>
+        <v>1800</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>118</v>
@@ -3134,24 +3139,19 @@
       </c>
       <c r="M55" s="10"/>
     </row>
-    <row r="56" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B56" s="24"/>
       <c r="C56" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="17">
-        <v>3</v>
-      </c>
-      <c r="E56" s="20">
-        <v>3285</v>
-      </c>
-      <c r="F56" s="18">
-        <f t="shared" si="4"/>
-        <v>9855</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E56" s="20"/>
+      <c r="F56" s="18"/>
       <c r="G56" s="5" t="s">
         <v>118</v>
       </c>
@@ -3164,23 +3164,23 @@
       </c>
       <c r="M56" s="10"/>
     </row>
-    <row r="57" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="B57" s="24"/>
       <c r="C57" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E57" s="20">
-        <v>7250</v>
+        <v>1840</v>
       </c>
       <c r="F57" s="18">
-        <f t="shared" si="4"/>
-        <v>7250</v>
+        <f t="shared" ref="F57:F62" si="6">E57*D57</f>
+        <v>3680</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>118</v>
@@ -3194,23 +3194,23 @@
       </c>
       <c r="M57" s="10"/>
     </row>
-    <row r="58" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B58" s="24"/>
       <c r="C58" s="4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D58" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E58" s="20">
-        <v>1150</v>
+        <v>592.22</v>
       </c>
       <c r="F58" s="18">
-        <f t="shared" si="4"/>
-        <v>4600</v>
+        <f t="shared" si="6"/>
+        <v>1184.44</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>118</v>
@@ -3224,23 +3224,23 @@
       </c>
       <c r="M58" s="10"/>
     </row>
-    <row r="59" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B59" s="24"/>
       <c r="C59" s="4" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D59" s="17">
         <v>6</v>
       </c>
-      <c r="E59" s="20">
-        <v>1220</v>
+      <c r="E59" s="18">
+        <v>3700</v>
       </c>
       <c r="F59" s="18">
-        <f t="shared" si="4"/>
-        <v>7320</v>
+        <f t="shared" si="6"/>
+        <v>22200</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>118</v>
@@ -3254,23 +3254,23 @@
       </c>
       <c r="M59" s="10"/>
     </row>
-    <row r="60" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B60" s="24"/>
       <c r="C60" s="4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D60" s="17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E60" s="20">
-        <v>11656</v>
+        <v>600</v>
       </c>
       <c r="F60" s="18">
-        <f t="shared" si="4"/>
-        <v>116560</v>
+        <f t="shared" si="6"/>
+        <v>600</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>118</v>
@@ -3284,23 +3284,21 @@
       </c>
       <c r="M60" s="10"/>
     </row>
-    <row r="61" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="B61" s="24"/>
       <c r="C61" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D61" s="17">
-        <v>1</v>
-      </c>
-      <c r="E61" s="20">
-        <v>5360</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E61" s="20"/>
       <c r="F61" s="18">
-        <f t="shared" si="4"/>
-        <v>5360</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>118</v>
@@ -3314,19 +3312,24 @@
       </c>
       <c r="M61" s="10"/>
     </row>
-    <row r="62" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="B62" s="24"/>
       <c r="C62" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D62" s="17">
         <v>1</v>
       </c>
-      <c r="E62" s="20"/>
-      <c r="F62" s="18"/>
+      <c r="E62" s="20">
+        <v>850</v>
+      </c>
+      <c r="F62" s="18">
+        <f t="shared" si="6"/>
+        <v>850</v>
+      </c>
       <c r="G62" s="5" t="s">
         <v>118</v>
       </c>
@@ -3339,24 +3342,29 @@
       </c>
       <c r="M62" s="10"/>
     </row>
-    <row r="63" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B63" s="24"/>
+        <v>91</v>
+      </c>
+      <c r="B63" s="11"/>
       <c r="C63" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="17">
-        <v>1</v>
-      </c>
-      <c r="E63" s="20"/>
-      <c r="F63" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="E63" s="18">
+        <v>210</v>
+      </c>
+      <c r="F63" s="18">
+        <f t="shared" ref="F63:F76" si="7">D63*E63</f>
+        <v>4200</v>
+      </c>
       <c r="G63" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I63" s="5"/>
       <c r="J63" s="5" t="s">
@@ -3364,24 +3372,29 @@
       </c>
       <c r="M63" s="10"/>
     </row>
-    <row r="64" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B64" s="24"/>
+        <v>92</v>
+      </c>
+      <c r="B64" s="11"/>
       <c r="C64" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D64" s="17">
-        <v>1</v>
-      </c>
-      <c r="E64" s="20"/>
-      <c r="F64" s="18"/>
+        <v>100</v>
+      </c>
+      <c r="E64" s="18">
+        <v>135</v>
+      </c>
+      <c r="F64" s="18">
+        <f t="shared" si="7"/>
+        <v>13500</v>
+      </c>
       <c r="G64" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I64" s="5"/>
       <c r="J64" s="5" t="s">
@@ -3389,24 +3402,29 @@
       </c>
       <c r="M64" s="10"/>
     </row>
-    <row r="65" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B65" s="24"/>
+        <v>93</v>
+      </c>
+      <c r="B65" s="11"/>
       <c r="C65" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="17">
-        <v>1</v>
-      </c>
-      <c r="E65" s="20"/>
-      <c r="F65" s="18"/>
+        <v>100</v>
+      </c>
+      <c r="E65" s="18">
+        <v>135</v>
+      </c>
+      <c r="F65" s="18">
+        <f t="shared" si="7"/>
+        <v>13500</v>
+      </c>
       <c r="G65" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I65" s="5"/>
       <c r="J65" s="5" t="s">
@@ -3414,29 +3432,29 @@
       </c>
       <c r="M65" s="10"/>
     </row>
-    <row r="66" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B66" s="24"/>
+        <v>94</v>
+      </c>
+      <c r="B66" s="11"/>
       <c r="C66" s="4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D66" s="17">
-        <v>6</v>
-      </c>
-      <c r="E66" s="20">
-        <v>11656</v>
+        <v>20</v>
+      </c>
+      <c r="E66" s="18">
+        <v>210</v>
       </c>
       <c r="F66" s="18">
-        <f t="shared" ref="F66:F74" si="5">E66*D66</f>
-        <v>69936</v>
+        <f t="shared" si="7"/>
+        <v>4200</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I66" s="5"/>
       <c r="J66" s="5" t="s">
@@ -3444,29 +3462,29 @@
       </c>
       <c r="M66" s="10"/>
     </row>
-    <row r="67" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B67" s="24"/>
+        <v>95</v>
+      </c>
+      <c r="B67" s="11"/>
       <c r="C67" s="4" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D67" s="17">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E67" s="18">
-        <v>21900</v>
+        <v>102</v>
       </c>
       <c r="F67" s="18">
-        <f t="shared" si="5"/>
-        <v>284700</v>
+        <f t="shared" si="7"/>
+        <v>1530</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I67" s="5"/>
       <c r="J67" s="5" t="s">
@@ -3474,29 +3492,29 @@
       </c>
       <c r="M67" s="10"/>
     </row>
-    <row r="68" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B68" s="24"/>
+        <v>96</v>
+      </c>
+      <c r="B68" s="11"/>
       <c r="C68" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D68" s="17">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E68" s="18">
-        <v>4700</v>
+        <v>500</v>
       </c>
       <c r="F68" s="18">
-        <f t="shared" si="5"/>
-        <v>9400</v>
+        <f t="shared" si="7"/>
+        <v>12500</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I68" s="5"/>
       <c r="J68" s="5" t="s">
@@ -3504,29 +3522,29 @@
       </c>
       <c r="M68" s="10"/>
     </row>
-    <row r="69" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B69" s="24"/>
+        <v>97</v>
+      </c>
+      <c r="B69" s="11"/>
       <c r="C69" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D69" s="17">
-        <v>4</v>
-      </c>
-      <c r="E69" s="20">
-        <v>3285</v>
+        <v>15</v>
+      </c>
+      <c r="E69" s="18">
+        <v>210</v>
       </c>
       <c r="F69" s="18">
-        <f t="shared" si="5"/>
-        <v>13140</v>
+        <f t="shared" si="7"/>
+        <v>3150</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I69" s="5"/>
       <c r="J69" s="5" t="s">
@@ -3534,29 +3552,29 @@
       </c>
       <c r="M69" s="10"/>
     </row>
-    <row r="70" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B70" s="24"/>
+        <v>98</v>
+      </c>
+      <c r="B70" s="11"/>
       <c r="C70" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" s="17">
+        <v>8</v>
+      </c>
+      <c r="D70" s="21">
+        <v>10</v>
+      </c>
+      <c r="E70" s="18">
         <v>25</v>
       </c>
-      <c r="E70" s="20">
-        <v>1150</v>
-      </c>
       <c r="F70" s="18">
-        <f t="shared" si="5"/>
-        <v>28750</v>
+        <f t="shared" si="7"/>
+        <v>250</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I70" s="5"/>
       <c r="J70" s="5" t="s">
@@ -3564,29 +3582,29 @@
       </c>
       <c r="M70" s="10"/>
     </row>
-    <row r="71" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B71" s="24"/>
+        <v>99</v>
+      </c>
+      <c r="B71" s="11"/>
       <c r="C71" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D71" s="17">
-        <v>14</v>
-      </c>
-      <c r="E71" s="20">
-        <v>1220</v>
+        <v>35</v>
+      </c>
+      <c r="E71" s="18">
+        <v>3000</v>
       </c>
       <c r="F71" s="18">
-        <f t="shared" si="5"/>
-        <v>17080</v>
+        <f t="shared" si="7"/>
+        <v>105000</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I71" s="5"/>
       <c r="J71" s="5" t="s">
@@ -3594,29 +3612,29 @@
       </c>
       <c r="M71" s="10"/>
     </row>
-    <row r="72" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" s="24"/>
+        <v>100</v>
+      </c>
+      <c r="B72" s="11"/>
       <c r="C72" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" s="17">
-        <v>10</v>
-      </c>
-      <c r="E72" s="20">
-        <v>180</v>
+        <v>7</v>
+      </c>
+      <c r="D72" s="21">
+        <v>2</v>
+      </c>
+      <c r="E72" s="18">
+        <v>2150</v>
       </c>
       <c r="F72" s="18">
-        <f t="shared" si="5"/>
-        <v>1800</v>
+        <f t="shared" si="7"/>
+        <v>4300</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I72" s="5"/>
       <c r="J72" s="5" t="s">
@@ -3624,29 +3642,29 @@
       </c>
       <c r="M72" s="10"/>
     </row>
-    <row r="73" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" s="24"/>
+        <v>101</v>
+      </c>
+      <c r="B73" s="11"/>
       <c r="C73" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D73" s="17">
-        <v>1</v>
-      </c>
-      <c r="E73" s="20">
-        <v>7250</v>
+      <c r="D73" s="21">
+        <v>2</v>
+      </c>
+      <c r="E73" s="18">
+        <v>500</v>
       </c>
       <c r="F73" s="18">
-        <f t="shared" si="5"/>
-        <v>7250</v>
+        <f t="shared" si="7"/>
+        <v>1000</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I73" s="5"/>
       <c r="J73" s="5" t="s">
@@ -3654,29 +3672,29 @@
       </c>
       <c r="M73" s="10"/>
     </row>
-    <row r="74" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B74" s="24"/>
+        <v>102</v>
+      </c>
+      <c r="B74" s="11"/>
       <c r="C74" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" s="17">
-        <v>1</v>
-      </c>
-      <c r="E74" s="20">
-        <v>8240</v>
+        <v>6</v>
+      </c>
+      <c r="D74" s="21">
+        <v>50</v>
+      </c>
+      <c r="E74" s="18">
+        <v>13</v>
       </c>
       <c r="F74" s="18">
-        <f t="shared" si="5"/>
-        <v>8240</v>
+        <f t="shared" si="7"/>
+        <v>650</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I74" s="5"/>
       <c r="J74" s="5" t="s">
@@ -3684,24 +3702,29 @@
       </c>
       <c r="M74" s="10"/>
     </row>
-    <row r="75" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B75" s="24"/>
+        <v>103</v>
+      </c>
+      <c r="B75" s="11"/>
       <c r="C75" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D75" s="17">
-        <v>1</v>
-      </c>
-      <c r="E75" s="20"/>
-      <c r="F75" s="18"/>
+      <c r="D75" s="21">
+        <v>50</v>
+      </c>
+      <c r="E75" s="18">
+        <v>13</v>
+      </c>
+      <c r="F75" s="18">
+        <f t="shared" si="7"/>
+        <v>650</v>
+      </c>
       <c r="G75" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I75" s="5"/>
       <c r="J75" s="5" t="s">
@@ -3709,29 +3732,29 @@
       </c>
       <c r="M75" s="10"/>
     </row>
-    <row r="76" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B76" s="24"/>
+        <v>104</v>
+      </c>
+      <c r="B76" s="11"/>
       <c r="C76" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D76" s="17">
-        <v>2</v>
-      </c>
-      <c r="E76" s="20">
-        <v>1840</v>
+      <c r="D76" s="21">
+        <v>20</v>
+      </c>
+      <c r="E76" s="18">
+        <v>205</v>
       </c>
       <c r="F76" s="18">
-        <f t="shared" ref="F76:F82" si="6">E76*D76</f>
-        <v>3680</v>
+        <f t="shared" si="7"/>
+        <v>4100</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I76" s="5"/>
       <c r="J76" s="5" t="s">
@@ -3739,29 +3762,29 @@
       </c>
       <c r="M76" s="10"/>
     </row>
-    <row r="77" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B77" s="24"/>
+        <v>105</v>
+      </c>
+      <c r="B77" s="11"/>
       <c r="C77" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D77" s="17">
+        <v>9</v>
+      </c>
+      <c r="D77" s="21">
         <v>2</v>
       </c>
-      <c r="E77" s="20">
-        <v>592.22</v>
+      <c r="E77" s="18">
+        <v>650</v>
       </c>
       <c r="F77" s="18">
-        <f t="shared" si="6"/>
-        <v>1184.44</v>
+        <f>D77*E77</f>
+        <v>1300</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="5" t="s">
@@ -3769,29 +3792,29 @@
       </c>
       <c r="M77" s="10"/>
     </row>
-    <row r="78" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B78" s="24"/>
+        <v>106</v>
+      </c>
+      <c r="B78" s="11"/>
       <c r="C78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D78" s="17">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="D78" s="21">
+        <v>1</v>
       </c>
       <c r="E78" s="18">
-        <v>3700</v>
+        <v>1380</v>
       </c>
       <c r="F78" s="18">
-        <f t="shared" si="6"/>
-        <v>22200</v>
+        <f>D78*E78</f>
+        <v>1380</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="5" t="s">
@@ -3799,29 +3822,29 @@
       </c>
       <c r="M78" s="10"/>
     </row>
-    <row r="79" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B79" s="24"/>
+        <v>107</v>
+      </c>
+      <c r="B79" s="11"/>
       <c r="C79" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="17">
+        <v>5</v>
+      </c>
+      <c r="D79" s="21">
         <v>1</v>
       </c>
-      <c r="E79" s="20">
-        <v>600</v>
+      <c r="E79" s="18">
+        <v>17121</v>
       </c>
       <c r="F79" s="18">
-        <f t="shared" si="6"/>
-        <v>600</v>
+        <f>D79*E79</f>
+        <v>17121</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I79" s="5"/>
       <c r="J79" s="5" t="s">
@@ -3829,27 +3852,31 @@
       </c>
       <c r="M79" s="10"/>
     </row>
-    <row r="80" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B80" s="24"/>
+        <v>108</v>
+      </c>
+      <c r="B80" s="11">
+        <v>1</v>
+      </c>
       <c r="C80" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D80" s="17">
-        <v>2</v>
-      </c>
-      <c r="E80" s="20"/>
+        <v>6</v>
+      </c>
+      <c r="E80" s="18">
+        <v>2563.54</v>
+      </c>
       <c r="F80" s="18">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>B80*D80*E80</f>
+        <v>15381.24</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I80" s="5"/>
       <c r="J80" s="5" t="s">
@@ -3857,29 +3884,31 @@
       </c>
       <c r="M80" s="10"/>
     </row>
-    <row r="81" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B81" s="24"/>
+        <v>109</v>
+      </c>
+      <c r="B81" s="11">
+        <v>1</v>
+      </c>
       <c r="C81" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D81" s="17">
-        <v>1</v>
-      </c>
-      <c r="E81" s="20">
-        <v>850</v>
+        <v>40</v>
+      </c>
+      <c r="E81" s="18">
+        <v>1695.62</v>
       </c>
       <c r="F81" s="18">
-        <f t="shared" si="6"/>
-        <v>850</v>
+        <f t="shared" ref="F81:F88" si="8">B81*D81*E81</f>
+        <v>67824.799999999988</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I81" s="5"/>
       <c r="J81" s="5" t="s">
@@ -3887,29 +3916,31 @@
       </c>
       <c r="M81" s="10"/>
     </row>
-    <row r="82" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B82" s="24"/>
+        <v>110</v>
+      </c>
+      <c r="B82" s="11">
+        <v>1</v>
+      </c>
       <c r="C82" s="4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D82" s="17">
-        <v>1</v>
-      </c>
-      <c r="E82" s="20">
-        <v>5000</v>
+        <v>40</v>
+      </c>
+      <c r="E82" s="18">
+        <v>1191</v>
       </c>
       <c r="F82" s="18">
-        <f t="shared" si="6"/>
-        <v>5000</v>
+        <f t="shared" si="8"/>
+        <v>47640</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I82" s="5"/>
       <c r="J82" s="5" t="s">
@@ -3917,29 +3948,31 @@
       </c>
       <c r="M82" s="10"/>
     </row>
-    <row r="83" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B83" s="11"/>
+        <v>111</v>
+      </c>
+      <c r="B83" s="11">
+        <v>1</v>
+      </c>
       <c r="C83" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D83" s="17">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E83" s="18">
-        <v>210</v>
+        <v>1498.6</v>
       </c>
       <c r="F83" s="18">
-        <f t="shared" ref="F83:F96" si="7">D83*E83</f>
-        <v>4200</v>
+        <f t="shared" si="8"/>
+        <v>59944</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I83" s="5"/>
       <c r="J83" s="5" t="s">
@@ -3947,29 +3980,31 @@
       </c>
       <c r="M83" s="10"/>
     </row>
-    <row r="84" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B84" s="11"/>
+        <v>112</v>
+      </c>
+      <c r="B84" s="11">
+        <v>1</v>
+      </c>
       <c r="C84" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D84" s="17">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E84" s="18">
-        <v>135</v>
+        <v>1498.6</v>
       </c>
       <c r="F84" s="18">
-        <f t="shared" si="7"/>
-        <v>13500</v>
+        <f t="shared" si="8"/>
+        <v>59944</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I84" s="5"/>
       <c r="J84" s="5" t="s">
@@ -3977,29 +4012,31 @@
       </c>
       <c r="M84" s="10"/>
     </row>
-    <row r="85" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B85" s="11"/>
+        <v>113</v>
+      </c>
+      <c r="B85" s="11">
+        <v>2</v>
+      </c>
       <c r="C85" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D85" s="17">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E85" s="18">
-        <v>135</v>
+        <v>1627.37</v>
       </c>
       <c r="F85" s="18">
-        <f t="shared" si="7"/>
-        <v>13500</v>
+        <f t="shared" si="8"/>
+        <v>130189.59999999999</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I85" s="5"/>
       <c r="J85" s="5" t="s">
@@ -4007,29 +4044,30 @@
       </c>
       <c r="M85" s="10"/>
     </row>
-    <row r="86" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B86" s="11"/>
+        <v>114</v>
+      </c>
+      <c r="B86" s="11">
+        <v>3</v>
+      </c>
       <c r="C86" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D86" s="17">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E86" s="18">
-        <v>210</v>
+        <v>1300</v>
       </c>
       <c r="F86" s="18">
-        <f t="shared" si="7"/>
-        <v>4200</v>
+        <v>156020.4</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I86" s="5"/>
       <c r="J86" s="5" t="s">
@@ -4037,29 +4075,30 @@
       </c>
       <c r="M86" s="10"/>
     </row>
-    <row r="87" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B87" s="11"/>
+        <v>115</v>
+      </c>
+      <c r="B87" s="11">
+        <v>7</v>
+      </c>
       <c r="C87" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D87" s="17">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E87" s="18">
-        <v>102</v>
+        <v>1031.77</v>
       </c>
       <c r="F87" s="18">
-        <f t="shared" si="7"/>
-        <v>1530</v>
+        <v>288894.40000000002</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I87" s="5"/>
       <c r="J87" s="5" t="s">
@@ -4067,29 +4106,31 @@
       </c>
       <c r="M87" s="10"/>
     </row>
-    <row r="88" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B88" s="11"/>
+        <v>116</v>
+      </c>
+      <c r="B88" s="4">
+        <v>1</v>
+      </c>
       <c r="C88" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D88" s="17">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E88" s="18">
-        <v>500</v>
+        <v>911.13</v>
       </c>
       <c r="F88" s="18">
-        <f t="shared" si="7"/>
-        <v>12500</v>
+        <f t="shared" si="8"/>
+        <v>36445.199999999997</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>118</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I88" s="5"/>
       <c r="J88" s="5" t="s">
@@ -4097,625 +4138,12 @@
       </c>
       <c r="M88" s="10"/>
     </row>
-    <row r="89" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B89" s="11"/>
-      <c r="C89" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" s="17">
-        <v>15</v>
-      </c>
-      <c r="E89" s="18">
-        <v>210</v>
-      </c>
-      <c r="F89" s="18">
-        <f t="shared" si="7"/>
-        <v>3150</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I89" s="5"/>
-      <c r="J89" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M89" s="10"/>
-    </row>
-    <row r="90" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B90" s="11"/>
-      <c r="C90" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90" s="21">
-        <v>10</v>
-      </c>
-      <c r="E90" s="18">
-        <v>25</v>
-      </c>
-      <c r="F90" s="18">
-        <f t="shared" si="7"/>
-        <v>250</v>
-      </c>
-      <c r="G90" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I90" s="5"/>
-      <c r="J90" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M90" s="10"/>
-    </row>
-    <row r="91" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B91" s="11"/>
-      <c r="C91" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D91" s="17">
-        <v>35</v>
-      </c>
-      <c r="E91" s="18">
-        <v>3000</v>
-      </c>
-      <c r="F91" s="18">
-        <f t="shared" si="7"/>
-        <v>105000</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H91" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I91" s="5"/>
-      <c r="J91" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M91" s="10"/>
-    </row>
-    <row r="92" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B92" s="11"/>
-      <c r="C92" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D92" s="21">
-        <v>2</v>
-      </c>
-      <c r="E92" s="18">
-        <v>2150</v>
-      </c>
-      <c r="F92" s="18">
-        <f t="shared" si="7"/>
-        <v>4300</v>
-      </c>
-      <c r="G92" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H92" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I92" s="5"/>
-      <c r="J92" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M92" s="10"/>
-    </row>
-    <row r="93" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B93" s="11"/>
-      <c r="C93" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" s="21">
-        <v>2</v>
-      </c>
-      <c r="E93" s="18">
-        <v>500</v>
-      </c>
-      <c r="F93" s="18">
-        <f t="shared" si="7"/>
-        <v>1000</v>
-      </c>
-      <c r="G93" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H93" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I93" s="5"/>
-      <c r="J93" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M93" s="10"/>
-    </row>
-    <row r="94" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B94" s="11"/>
-      <c r="C94" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D94" s="21">
-        <v>50</v>
-      </c>
-      <c r="E94" s="18">
-        <v>13</v>
-      </c>
-      <c r="F94" s="18">
-        <f t="shared" si="7"/>
-        <v>650</v>
-      </c>
-      <c r="G94" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I94" s="5"/>
-      <c r="J94" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M94" s="10"/>
-    </row>
-    <row r="95" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B95" s="11"/>
-      <c r="C95" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D95" s="21">
-        <v>50</v>
-      </c>
-      <c r="E95" s="18">
-        <v>13</v>
-      </c>
-      <c r="F95" s="18">
-        <f t="shared" si="7"/>
-        <v>650</v>
-      </c>
-      <c r="G95" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H95" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I95" s="5"/>
-      <c r="J95" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M95" s="10"/>
-    </row>
-    <row r="96" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B96" s="11"/>
-      <c r="C96" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D96" s="21">
-        <v>20</v>
-      </c>
-      <c r="E96" s="18">
-        <v>205</v>
-      </c>
-      <c r="F96" s="18">
-        <f t="shared" si="7"/>
-        <v>4100</v>
-      </c>
-      <c r="G96" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H96" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I96" s="5"/>
-      <c r="J96" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M96" s="10"/>
-    </row>
-    <row r="97" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B97" s="11"/>
-      <c r="C97" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D97" s="21">
-        <v>2</v>
-      </c>
-      <c r="E97" s="18">
-        <v>650</v>
-      </c>
-      <c r="F97" s="18">
-        <f>D97*E97</f>
-        <v>1300</v>
-      </c>
-      <c r="G97" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H97" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I97" s="5"/>
-      <c r="J97" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M97" s="10"/>
-    </row>
-    <row r="98" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B98" s="11"/>
-      <c r="C98" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D98" s="21">
-        <v>1</v>
-      </c>
-      <c r="E98" s="18">
-        <v>1380</v>
-      </c>
-      <c r="F98" s="18">
-        <f>D98*E98</f>
-        <v>1380</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H98" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I98" s="5"/>
-      <c r="J98" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M98" s="10"/>
-    </row>
-    <row r="99" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B99" s="11"/>
-      <c r="C99" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99" s="21">
-        <v>1</v>
-      </c>
-      <c r="E99" s="18">
-        <v>17121</v>
-      </c>
-      <c r="F99" s="18">
-        <f>D99*E99</f>
-        <v>17121</v>
-      </c>
-      <c r="G99" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H99" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I99" s="5"/>
-      <c r="J99" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M99" s="10"/>
-    </row>
-    <row r="100" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B100" s="11">
-        <v>1</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D100" s="17">
-        <v>6</v>
-      </c>
-      <c r="E100" s="18">
-        <v>2563.54</v>
-      </c>
-      <c r="F100" s="18">
-        <f>B100*D100*E100</f>
-        <v>15381.24</v>
-      </c>
-      <c r="G100" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H100" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I100" s="5"/>
-      <c r="J100" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M100" s="10"/>
-    </row>
-    <row r="101" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B101" s="11">
-        <v>1</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D101" s="17">
-        <v>40</v>
-      </c>
-      <c r="E101" s="18">
-        <v>1695.62</v>
-      </c>
-      <c r="F101" s="18">
-        <f t="shared" ref="F101:F108" si="8">B101*D101*E101</f>
-        <v>67824.799999999988</v>
-      </c>
-      <c r="G101" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H101" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I101" s="5"/>
-      <c r="J101" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M101" s="10"/>
-    </row>
-    <row r="102" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B102" s="11">
-        <v>1</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D102" s="17">
-        <v>40</v>
-      </c>
-      <c r="E102" s="18">
-        <v>1191</v>
-      </c>
-      <c r="F102" s="18">
-        <f t="shared" si="8"/>
-        <v>47640</v>
-      </c>
-      <c r="G102" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H102" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I102" s="5"/>
-      <c r="J102" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M102" s="10"/>
-    </row>
-    <row r="103" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B103" s="11">
-        <v>1</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D103" s="17">
-        <v>40</v>
-      </c>
-      <c r="E103" s="18">
-        <v>1498.6</v>
-      </c>
-      <c r="F103" s="18">
-        <f t="shared" si="8"/>
-        <v>59944</v>
-      </c>
-      <c r="G103" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H103" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I103" s="5"/>
-      <c r="J103" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M103" s="10"/>
-    </row>
-    <row r="104" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B104" s="11">
-        <v>1</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D104" s="17">
-        <v>40</v>
-      </c>
-      <c r="E104" s="18">
-        <v>1498.6</v>
-      </c>
-      <c r="F104" s="18">
-        <f t="shared" si="8"/>
-        <v>59944</v>
-      </c>
-      <c r="G104" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H104" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I104" s="5"/>
-      <c r="J104" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M104" s="10"/>
-    </row>
-    <row r="105" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B105" s="11">
-        <v>2</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D105" s="17">
-        <v>40</v>
-      </c>
-      <c r="E105" s="18">
-        <v>1627.37</v>
-      </c>
-      <c r="F105" s="18">
-        <f t="shared" si="8"/>
-        <v>130189.59999999999</v>
-      </c>
-      <c r="G105" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H105" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I105" s="5"/>
-      <c r="J105" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M105" s="10"/>
-    </row>
-    <row r="106" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B106" s="11">
-        <v>3</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D106" s="17">
-        <v>40</v>
-      </c>
-      <c r="E106" s="18">
-        <v>1300</v>
-      </c>
-      <c r="F106" s="18">
-        <v>156020.4</v>
-      </c>
-      <c r="G106" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H106" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I106" s="5"/>
-      <c r="J106" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M106" s="10"/>
-    </row>
-    <row r="107" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B107" s="11">
-        <v>7</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D107" s="17">
-        <v>40</v>
-      </c>
-      <c r="E107" s="18">
-        <v>1031.77</v>
-      </c>
-      <c r="F107" s="18">
-        <v>288894.40000000002</v>
-      </c>
-      <c r="G107" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H107" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I107" s="5"/>
-      <c r="J107" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M107" s="10"/>
-    </row>
-    <row r="108" spans="1:13" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B108" s="4">
-        <v>1</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D108" s="17">
-        <v>40</v>
-      </c>
-      <c r="E108" s="18">
-        <v>911.13</v>
-      </c>
-      <c r="F108" s="18">
-        <f t="shared" si="8"/>
-        <v>36445.199999999997</v>
-      </c>
-      <c r="G108" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H108" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I108" s="5"/>
-      <c r="J108" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M108" s="10"/>
-    </row>
-    <row r="109" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:O1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:O1"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>
   <pageSetup paperSize="8" scale="42" orientation="portrait" r:id="rId1"/>
@@ -4724,81 +4152,81 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Clean duplicated item names
</commit_message>
<xml_diff>
--- a/data/quotation_princing_analysis/INDEPENDENT CIP EVAPORATOR CIR RETURN LINE GOING TO IS 400M3 TANK - ACEPACK.xlsx
+++ b/data/quotation_princing_analysis/INDEPENDENT CIP EVAPORATOR CIR RETURN LINE GOING TO IS 400M3 TANK - ACEPACK.xlsx
@@ -1038,7 +1038,27 @@
     <cellStyle name="Total" xfId="50" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="51" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1497,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2519,7 +2539,7 @@
         <v>11656</v>
       </c>
       <c r="F34" s="18">
-        <f>E34*D34</f>
+        <f t="shared" ref="F34:F39" si="4">E34*D34</f>
         <v>46624</v>
       </c>
       <c r="G34" s="5" t="s">
@@ -2549,7 +2569,7 @@
         <v>1500</v>
       </c>
       <c r="F35" s="18">
-        <f>E35*D35</f>
+        <f t="shared" si="4"/>
         <v>1500</v>
       </c>
       <c r="G35" s="5" t="s">
@@ -2579,7 +2599,7 @@
         <v>1150</v>
       </c>
       <c r="F36" s="18">
-        <f>E36*D36</f>
+        <f t="shared" si="4"/>
         <v>16100</v>
       </c>
       <c r="G36" s="5" t="s">
@@ -2609,7 +2629,7 @@
         <v>27384</v>
       </c>
       <c r="F37" s="18">
-        <f>E37*D37</f>
+        <f t="shared" si="4"/>
         <v>82152</v>
       </c>
       <c r="G37" s="5" t="s">
@@ -2639,7 +2659,7 @@
         <v>35000</v>
       </c>
       <c r="F38" s="18">
-        <f>E38*D38</f>
+        <f t="shared" si="4"/>
         <v>35000</v>
       </c>
       <c r="G38" s="5" t="s">
@@ -2669,7 +2689,7 @@
         <v>26500</v>
       </c>
       <c r="F39" s="18">
-        <f>E39*D39</f>
+        <f t="shared" si="4"/>
         <v>79500</v>
       </c>
       <c r="G39" s="5" t="s">
@@ -2779,7 +2799,7 @@
         <v>21900</v>
       </c>
       <c r="F43" s="18">
-        <f t="shared" ref="F43:F45" si="4">E43*D43</f>
+        <f t="shared" ref="F43:F45" si="5">E43*D43</f>
         <v>219000</v>
       </c>
       <c r="G43" s="5" t="s">
@@ -2809,7 +2829,7 @@
         <v>3285</v>
       </c>
       <c r="F44" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9855</v>
       </c>
       <c r="G44" s="5" t="s">
@@ -2839,7 +2859,7 @@
         <v>1220</v>
       </c>
       <c r="F45" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7320</v>
       </c>
       <c r="G45" s="5" t="s">
@@ -2944,7 +2964,7 @@
         <v>11656</v>
       </c>
       <c r="F49" s="18">
-        <f t="shared" ref="F49:F55" si="5">E49*D49</f>
+        <f t="shared" ref="F49:F55" si="6">E49*D49</f>
         <v>69936</v>
       </c>
       <c r="G49" s="5" t="s">
@@ -2974,7 +2994,7 @@
         <v>21900</v>
       </c>
       <c r="F50" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>284700</v>
       </c>
       <c r="G50" s="5" t="s">
@@ -3004,7 +3024,7 @@
         <v>4700</v>
       </c>
       <c r="F51" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9400</v>
       </c>
       <c r="G51" s="5" t="s">
@@ -3034,7 +3054,7 @@
         <v>3285</v>
       </c>
       <c r="F52" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13140</v>
       </c>
       <c r="G52" s="5" t="s">
@@ -3064,7 +3084,7 @@
         <v>1150</v>
       </c>
       <c r="F53" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28750</v>
       </c>
       <c r="G53" s="5" t="s">
@@ -3094,7 +3114,7 @@
         <v>1220</v>
       </c>
       <c r="F54" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17080</v>
       </c>
       <c r="G54" s="5" t="s">
@@ -3124,7 +3144,7 @@
         <v>180</v>
       </c>
       <c r="F55" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1800</v>
       </c>
       <c r="G55" s="5" t="s">
@@ -3179,7 +3199,7 @@
         <v>1840</v>
       </c>
       <c r="F57" s="18">
-        <f t="shared" ref="F57:F62" si="6">E57*D57</f>
+        <f t="shared" ref="F57:F62" si="7">E57*D57</f>
         <v>3680</v>
       </c>
       <c r="G57" s="5" t="s">
@@ -3209,7 +3229,7 @@
         <v>592.22</v>
       </c>
       <c r="F58" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1184.44</v>
       </c>
       <c r="G58" s="5" t="s">
@@ -3239,7 +3259,7 @@
         <v>3700</v>
       </c>
       <c r="F59" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>22200</v>
       </c>
       <c r="G59" s="5" t="s">
@@ -3269,7 +3289,7 @@
         <v>600</v>
       </c>
       <c r="F60" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>600</v>
       </c>
       <c r="G60" s="5" t="s">
@@ -3297,7 +3317,7 @@
       </c>
       <c r="E61" s="20"/>
       <c r="F61" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G61" s="5" t="s">
@@ -3327,7 +3347,7 @@
         <v>850</v>
       </c>
       <c r="F62" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>850</v>
       </c>
       <c r="G62" s="5" t="s">
@@ -3357,7 +3377,7 @@
         <v>210</v>
       </c>
       <c r="F63" s="18">
-        <f t="shared" ref="F63:F76" si="7">D63*E63</f>
+        <f t="shared" ref="F63:F76" si="8">D63*E63</f>
         <v>4200</v>
       </c>
       <c r="G63" s="5" t="s">
@@ -3387,7 +3407,7 @@
         <v>135</v>
       </c>
       <c r="F64" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13500</v>
       </c>
       <c r="G64" s="5" t="s">
@@ -3417,7 +3437,7 @@
         <v>135</v>
       </c>
       <c r="F65" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13500</v>
       </c>
       <c r="G65" s="5" t="s">
@@ -3447,7 +3467,7 @@
         <v>210</v>
       </c>
       <c r="F66" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4200</v>
       </c>
       <c r="G66" s="5" t="s">
@@ -3477,7 +3497,7 @@
         <v>102</v>
       </c>
       <c r="F67" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1530</v>
       </c>
       <c r="G67" s="5" t="s">
@@ -3507,7 +3527,7 @@
         <v>500</v>
       </c>
       <c r="F68" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12500</v>
       </c>
       <c r="G68" s="5" t="s">
@@ -3537,7 +3557,7 @@
         <v>210</v>
       </c>
       <c r="F69" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3150</v>
       </c>
       <c r="G69" s="5" t="s">
@@ -3567,7 +3587,7 @@
         <v>25</v>
       </c>
       <c r="F70" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>250</v>
       </c>
       <c r="G70" s="5" t="s">
@@ -3597,7 +3617,7 @@
         <v>3000</v>
       </c>
       <c r="F71" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>105000</v>
       </c>
       <c r="G71" s="5" t="s">
@@ -3627,7 +3647,7 @@
         <v>2150</v>
       </c>
       <c r="F72" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4300</v>
       </c>
       <c r="G72" s="5" t="s">
@@ -3657,7 +3677,7 @@
         <v>500</v>
       </c>
       <c r="F73" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1000</v>
       </c>
       <c r="G73" s="5" t="s">
@@ -3687,7 +3707,7 @@
         <v>13</v>
       </c>
       <c r="F74" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>650</v>
       </c>
       <c r="G74" s="5" t="s">
@@ -3717,7 +3737,7 @@
         <v>13</v>
       </c>
       <c r="F75" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>650</v>
       </c>
       <c r="G75" s="5" t="s">
@@ -3747,7 +3767,7 @@
         <v>205</v>
       </c>
       <c r="F76" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4100</v>
       </c>
       <c r="G76" s="5" t="s">
@@ -3901,7 +3921,7 @@
         <v>1695.62</v>
       </c>
       <c r="F81" s="18">
-        <f t="shared" ref="F81:F88" si="8">B81*D81*E81</f>
+        <f t="shared" ref="F81:F88" si="9">B81*D81*E81</f>
         <v>67824.799999999988</v>
       </c>
       <c r="G81" s="5" t="s">
@@ -3933,7 +3953,7 @@
         <v>1191</v>
       </c>
       <c r="F82" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>47640</v>
       </c>
       <c r="G82" s="5" t="s">
@@ -3965,7 +3985,7 @@
         <v>1498.6</v>
       </c>
       <c r="F83" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>59944</v>
       </c>
       <c r="G83" s="5" t="s">
@@ -3997,7 +4017,7 @@
         <v>1498.6</v>
       </c>
       <c r="F84" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>59944</v>
       </c>
       <c r="G84" s="5" t="s">
@@ -4029,7 +4049,7 @@
         <v>1627.37</v>
       </c>
       <c r="F85" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>130189.59999999999</v>
       </c>
       <c r="G85" s="5" t="s">
@@ -4123,7 +4143,7 @@
         <v>911.13</v>
       </c>
       <c r="F88" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>36445.199999999997</v>
       </c>
       <c r="G88" s="5" t="s">
@@ -4142,7 +4162,8 @@
   </sheetData>
   <autoFilter ref="A1:O1"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>

</xml_diff>